<commit_message>
Updated convert_to_dict function and plotting functions
</commit_message>
<xml_diff>
--- a/data/PV_spec.xlsx
+++ b/data/PV_spec.xlsx
@@ -432,7 +432,7 @@
     <col min="6" max="6" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="5" width="12.005" customWidth="1" bestFit="1"/>
     <col min="10" max="10" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
@@ -496,7 +496,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="4">
-        <v>400</v>
+        <v>800</v>
       </c>
       <c r="B4" s="3">
         <v>39.5</v>
@@ -511,16 +511,16 @@
         <v>9.07</v>
       </c>
       <c r="F4" s="3">
-        <v>0.23</v>
+        <v>0.28</v>
       </c>
       <c r="G4" s="4">
-        <v>400</v>
+        <v>5000</v>
       </c>
       <c r="H4" s="3">
-        <v>1.7</v>
-      </c>
-      <c r="I4" s="4">
-        <v>1</v>
+        <v>2.4</v>
+      </c>
+      <c r="I4" s="3">
+        <v>1.3</v>
       </c>
       <c r="J4" s="3">
         <v>-0.39</v>

</xml_diff>